<commit_message>
(feature) : fix upload template
</commit_message>
<xml_diff>
--- a/public/template/excel/template.xlsx
+++ b/public/template/excel/template.xlsx
@@ -5,36 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizdhan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizdhan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A80BA-4573-4C09-8F34-44A3074911FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34116AE4-0D4B-4F88-98B8-E1E78F87AFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{48482C42-A726-4C54-9547-D22DA1E59E76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bank_name" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>MOBILE_NUM</t>
   </si>
@@ -45,12 +37,6 @@
     <t>BANK_BR_CODE (OPTIONAL)</t>
   </si>
   <si>
-    <t>PRODUCT_NAME  (OPTIONAL)</t>
-  </si>
-  <si>
-    <t>BANK_NAME  (OPTIONAL)</t>
-  </si>
-  <si>
     <t>BANK_ACCOUNT</t>
   </si>
   <si>
@@ -60,28 +46,249 @@
     <t>NOMINAL</t>
   </si>
   <si>
-    <t>082338938580</t>
-  </si>
-  <si>
-    <t>00123456</t>
-  </si>
-  <si>
     <t>PRM100</t>
   </si>
   <si>
-    <t>BCA</t>
-  </si>
-  <si>
-    <t>Rendra</t>
+    <t>PRODUCT_NAME (OPTIONAL)</t>
+  </si>
+  <si>
+    <t>BANK_NAME (OPTIONAL)</t>
+  </si>
+  <si>
+    <t>BANK ANZ INDONESIA</t>
+  </si>
+  <si>
+    <t>BANK BJB SYARIAH</t>
+  </si>
+  <si>
+    <t>BANK BTPN</t>
+  </si>
+  <si>
+    <t>Bank Central Asia</t>
+  </si>
+  <si>
+    <t>BANK CTBC INDONESIA</t>
+  </si>
+  <si>
+    <t>BANK HARDA INTERNASIONAL</t>
+  </si>
+  <si>
+    <t>Bank Jago</t>
+  </si>
+  <si>
+    <t>Bank Mandiri</t>
+  </si>
+  <si>
+    <t>BANK MAYBANK INDONESIA</t>
+  </si>
+  <si>
+    <t>BANK MNC INTERNASIONAL</t>
+  </si>
+  <si>
+    <t>BANK MULTIARTA SENTOSA</t>
+  </si>
+  <si>
+    <t>Bank Negara Indonesia</t>
+  </si>
+  <si>
+    <t>BANK PANIN</t>
+  </si>
+  <si>
+    <t>Bank Permata</t>
+  </si>
+  <si>
+    <t>BANK QNB INDONESIA</t>
+  </si>
+  <si>
+    <t>Bank Rakyat Indonesia</t>
+  </si>
+  <si>
+    <t>BANK SAHABAT SAMPOERNA</t>
+  </si>
+  <si>
+    <t>BPD ACEH SYARIAH</t>
+  </si>
+  <si>
+    <t>BPD BALI</t>
+  </si>
+  <si>
+    <t>BPD BJB</t>
+  </si>
+  <si>
+    <t>BPD JAMBI</t>
+  </si>
+  <si>
+    <t>BPD JAWA TIMUR</t>
+  </si>
+  <si>
+    <t>BPD KALIMANTAN SELATAN</t>
+  </si>
+  <si>
+    <t>BPD KALIMANTAN TENGAH</t>
+  </si>
+  <si>
+    <t>BPD LAMPUNG</t>
+  </si>
+  <si>
+    <t>BPD NUSA TENGGARA TIMUR</t>
+  </si>
+  <si>
+    <t>BPD PAPUA</t>
+  </si>
+  <si>
+    <t>BPD RIAU KEPRI</t>
+  </si>
+  <si>
+    <t>BPD SUMATERA UTARA</t>
+  </si>
+  <si>
+    <t>BPD SUMSEL DAN BABEL</t>
+  </si>
+  <si>
+    <t>PT BANK DANAMON INDONESIA Tbk</t>
+  </si>
+  <si>
+    <t>PT BANK HSBC INDONESIA</t>
+  </si>
+  <si>
+    <t>PT BANK SEABANK INDONESIA</t>
+  </si>
+  <si>
+    <t>PT BANK SHINHAN INDONESIA</t>
+  </si>
+  <si>
+    <t>PT BANK SYARIAH INDONESIA TBK</t>
+  </si>
+  <si>
+    <t>PT. ALLO BANK INDONESIA TBK</t>
+  </si>
+  <si>
+    <t>PT. BANK ARTHA GRAHA INTERNASIONAL</t>
+  </si>
+  <si>
+    <t>PT. BANK BCA SYARIAH</t>
+  </si>
+  <si>
+    <t>PT. BANK CAPITAL INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK CIMB NIAGA Tbk.</t>
+  </si>
+  <si>
+    <t>PT. BANK COMMONWEALTH</t>
+  </si>
+  <si>
+    <t>PT. BANK DBS INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK DIGITAL BCA</t>
+  </si>
+  <si>
+    <t>PT. BANK GANESHA</t>
+  </si>
+  <si>
+    <t>PT. BANK ICBC INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK INA PERDANA</t>
+  </si>
+  <si>
+    <t>PT. BANK JASA JAKARTA</t>
+  </si>
+  <si>
+    <t>PT. BANK MASPION INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK MAYAPADA</t>
+  </si>
+  <si>
+    <t>PT. BANK MEGA Tbk.</t>
+  </si>
+  <si>
+    <t>PT. BANK MUAMALAT INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK NATIONALNOBU</t>
+  </si>
+  <si>
+    <t>PT. BANK NEO COMMERCE</t>
+  </si>
+  <si>
+    <t>PT. BANK OCBC NISP Tbk.</t>
+  </si>
+  <si>
+    <t>PT. BANK RESONA PERDANIA</t>
+  </si>
+  <si>
+    <t>PT. BANK SBI INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK SINARMAS</t>
+  </si>
+  <si>
+    <t>PT. BANK SYARIAH MEGA INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK TABUNGAN NEGARA (Persero)</t>
+  </si>
+  <si>
+    <t>PT. BANK UOB INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BANK WOORI SAUDARA INDONESIA</t>
+  </si>
+  <si>
+    <t>PT. BPD BENGKULU</t>
+  </si>
+  <si>
+    <t>PT. BPD DKI JAKARTA</t>
+  </si>
+  <si>
+    <t>PT. BPD MALUKU DAN MALUKU UTARA</t>
+  </si>
+  <si>
+    <t>PT. BUKOPIN</t>
+  </si>
+  <si>
+    <t>PT. SUPER BANK INDONESIA</t>
+  </si>
+  <si>
+    <t>PT.BPD KALTIM DAN KALTARA</t>
+  </si>
+  <si>
+    <t>STANDARD CHARTERED BANK</t>
+  </si>
+  <si>
+    <t>CITIBANK NA</t>
+  </si>
+  <si>
+    <t>OVO</t>
+  </si>
+  <si>
+    <t>DANA</t>
+  </si>
+  <si>
+    <t>GOPAY</t>
+  </si>
+  <si>
+    <t>SHOPEE</t>
+  </si>
+  <si>
+    <t>081233362015</t>
+  </si>
+  <si>
+    <t>00129090</t>
+  </si>
+  <si>
+    <t>Rendra 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -149,12 +356,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -473,71 +682,473 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="27.54296875" customWidth="1"/>
     <col min="4" max="4" width="34.1796875" customWidth="1"/>
-    <col min="5" max="5" width="27.36328125" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="18.90625" customWidth="1"/>
-    <col min="8" max="8" width="26.7265625" customWidth="1"/>
+    <col min="5" max="5" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="26.7265625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
+      <c r="A2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4">
+        <v>12330922231</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54395CE7-9D81-4BFA-8190-A2252A7BB464}">
+          <x14:formula1>
+            <xm:f>bank_name!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DB0FAC9-85AB-4BEE-99B8-D65DC928656F}">
+          <x14:formula1>
+            <xm:f>bank_name!$A$1:$A$68</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C70EF3-C35A-490C-BC3E-3A130DFFACC8}">
+  <dimension ref="A1:A73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>5610256645</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>5000000</v>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(feature) : add new validation for phone_num, change excel template, add new download report
</commit_message>
<xml_diff>
--- a/public/template/excel/template.xlsx
+++ b/public/template/excel/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizdhan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Laravel\DanamonUpload\public\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34116AE4-0D4B-4F88-98B8-E1E78F87AFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54720666-3A8E-441C-ACD9-A806C25B25EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{48482C42-A726-4C54-9547-D22DA1E59E76}"/>
   </bookViews>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>MOBILE_NUM</t>
   </si>
   <si>
-    <t>POL_NUM</t>
-  </si>
-  <si>
     <t>BANK_BR_CODE (OPTIONAL)</t>
   </si>
   <si>
@@ -46,15 +43,9 @@
     <t>NOMINAL</t>
   </si>
   <si>
-    <t>PRM100</t>
-  </si>
-  <si>
     <t>PRODUCT_NAME (OPTIONAL)</t>
   </si>
   <si>
-    <t>BANK_NAME (OPTIONAL)</t>
-  </si>
-  <si>
     <t>BANK ANZ INDONESIA</t>
   </si>
   <si>
@@ -274,13 +265,10 @@
     <t>SHOPEE</t>
   </si>
   <si>
-    <t>081233362015</t>
-  </si>
-  <si>
-    <t>00129090</t>
-  </si>
-  <si>
-    <t>Rendra 1</t>
+    <t>BANK_NAME</t>
+  </si>
+  <si>
+    <t>POL_NUM (OPTIONAL)</t>
   </si>
 </sst>
 </file>
@@ -682,7 +670,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,8 +678,7 @@
     <col min="1" max="1" width="21.453125" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.81640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="34.1796875" customWidth="1"/>
-    <col min="5" max="5" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.1796875" customWidth="1"/>
     <col min="6" max="6" width="21" style="4" customWidth="1"/>
     <col min="7" max="7" width="18.81640625" customWidth="1"/>
     <col min="8" max="8" width="26.7265625" style="6" customWidth="1"/>
@@ -702,68 +689,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4">
-        <v>12330922231</v>
-      </c>
-      <c r="G2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="6">
-        <v>5000000</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54395CE7-9D81-4BFA-8190-A2252A7BB464}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F1FC6A5-62E1-4D4B-A7D1-A1D9240ECE9F}">
           <x14:formula1>
-            <xm:f>bank_name!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9DB0FAC9-85AB-4BEE-99B8-D65DC928656F}">
-          <x14:formula1>
-            <xm:f>bank_name!$A$1:$A$68</xm:f>
+            <xm:f>bank_name!$A$1:$A$73</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
@@ -777,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C70EF3-C35A-490C-BC3E-3A130DFFACC8}">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -788,367 +747,367 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>